<commit_message>
Updated report with bugs
</commit_message>
<xml_diff>
--- a/Traceability Matrix.xlsx
+++ b/Traceability Matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Documents\GitHub\Advanced-Translation-Technology-Systems-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA56CD27-F659-494E-8ABE-299777C84BFE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B606D5F4-883B-47BD-9C42-05C745EFDA28}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CAFECA4A-9C9B-48C4-9EA0-A3B575DB3461}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="186">
   <si>
     <t>File Name</t>
   </si>
@@ -573,14 +573,71 @@
     <t>everything-core.xlf</t>
   </si>
   <si>
-    <t>N/A</t>
+    <t>Translated files (Memesource)</t>
+  </si>
+  <si>
+    <t>T.mxliff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Summary </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Summary</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SUMMARY</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -590,6 +647,15 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -623,11 +689,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -643,6 +710,527 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1234440</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0FE1E2FC-7B8F-4D3F-8CA5-00C89087E5FE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="53340" y="3787140"/>
+          <a:ext cx="8382000" cy="579120"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1100"/>
+            <a:t>Here all the files were translated using trados from xlf to xlf.sdlxliff.xlf .</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1100" baseline="0"/>
+            <a:t> This in turn produced files which were translated, however since they were now converted to version 1.2, they were not backwards compatable with our validation methods, as a result we could not validate same.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-IE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2491740</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C390668-9E61-4BBB-B1B0-F99F44EF22C9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22860" y="6088380"/>
+          <a:ext cx="9669780" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1100" b="0" u="none"/>
+            <a:t>Here</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t> we used trados to make our .xlf.sdlxliff.xlf into rich text format, we could not valiate same as our valiation methods were not backwards compatable </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-IE" sz="1100" b="0" u="none"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
+      <xdr:row>186</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2491740</xdr:colOff>
+      <xdr:row>188</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F41EF11-D514-418C-B239-65774DA6BFE5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="30480" y="33467040"/>
+          <a:ext cx="9662160" cy="533400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1100"/>
+            <a:t>Here</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1100" baseline="0"/>
+            <a:t> the Oasis SVN files were validated agaisnt already valid files as a controll in order to ensure our validation methods were in full working order. The results returned were as expected and all files were returned as valid.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-IE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>198</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2476500</xdr:colOff>
+      <xdr:row>201</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="TextBox 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53D13C24-1CEC-4D10-AF27-F7FA065A5FE4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22860" y="35661600"/>
+          <a:ext cx="9654540" cy="556260"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Here all the files were translated using Memsource from xlf to T.mxliff .</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> This in turn produced files which were translated, however unlike trados, these files were able to be validated by our validation methods as they were not converted to an older version. Overall, we found Memsource to be both a better and more efficent tool than trados.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-IE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>158</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2453640</xdr:colOff>
+      <xdr:row>160</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="TextBox 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1407C123-6A71-4231-8AD7-444731936D24}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="38100" y="28757880"/>
+          <a:ext cx="9616440" cy="434340"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Here</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> the Oasis SVN files were validated agaisnt already invalid files as a controll in order to ensure our validation methods were in full working order, the results were returned as expected and all files returned were invalid</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-IE">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-IE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>853440</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="TextBox 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91E21C94-AA8A-4CF9-8E3A-6C4A4BE3EF02}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="38100" y="1836420"/>
+          <a:ext cx="8016240" cy="358140"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1100"/>
+            <a:t>Here, all files were succesfully chnaged from HTML to XLF and no errors or inconveniences occurred</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -942,11 +1530,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0429365-BDE9-4319-B908-D2DFEABB6294}">
-  <dimension ref="A1:E175"/>
+  <dimension ref="A1:E198"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F180" sqref="F180"/>
+      <pane ySplit="1" topLeftCell="A191" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1099,35 +1687,26 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" t="s">
-        <v>21</v>
-      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
         <v>9</v>
@@ -1144,7 +1723,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
         <v>9</v>
@@ -1161,7 +1740,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
         <v>9</v>
@@ -1178,7 +1757,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
         <v>9</v>
@@ -1195,7 +1774,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
         <v>9</v>
@@ -1212,7 +1791,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
         <v>9</v>
@@ -1227,103 +1806,40 @@
         <v>21</v>
       </c>
     </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" t="s">
+        <v>21</v>
+      </c>
+    </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1" t="s">
+      <c r="A21" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" t="s">
-        <v>25</v>
-      </c>
-      <c r="D22" t="s">
-        <v>21</v>
-      </c>
-      <c r="E22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" t="s">
-        <v>33</v>
-      </c>
-      <c r="C23" t="s">
-        <v>25</v>
-      </c>
-      <c r="D23" t="s">
-        <v>21</v>
-      </c>
-      <c r="E23" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>28</v>
-      </c>
-      <c r="B24" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" t="s">
-        <v>25</v>
-      </c>
-      <c r="D24" t="s">
-        <v>21</v>
-      </c>
-      <c r="E24" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" t="s">
-        <v>33</v>
-      </c>
-      <c r="C25" t="s">
-        <v>25</v>
-      </c>
-      <c r="D25" t="s">
-        <v>21</v>
-      </c>
-      <c r="E25" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26" t="s">
-        <v>33</v>
-      </c>
-      <c r="C26" t="s">
-        <v>25</v>
-      </c>
-      <c r="D26" t="s">
-        <v>21</v>
-      </c>
-      <c r="E26" t="s">
-        <v>21</v>
-      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>33</v>
@@ -1340,7 +1856,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
         <v>33</v>
@@ -1355,154 +1871,108 @@
         <v>21</v>
       </c>
     </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" t="s">
+        <v>21</v>
+      </c>
+      <c r="E29" t="s">
+        <v>21</v>
+      </c>
+    </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" t="s">
+        <v>25</v>
+      </c>
+      <c r="D30" t="s">
+        <v>21</v>
+      </c>
+      <c r="E30" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="C31" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="D31" t="s">
         <v>21</v>
       </c>
       <c r="E31" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="C32" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="D32" t="s">
         <v>21</v>
       </c>
       <c r="E32" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="C33" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="D33" t="s">
         <v>21</v>
       </c>
       <c r="E33" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>38</v>
-      </c>
-      <c r="B34" t="s">
-        <v>9</v>
-      </c>
-      <c r="C34" t="s">
-        <v>9</v>
-      </c>
-      <c r="D34" t="s">
-        <v>21</v>
-      </c>
-      <c r="E34" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>39</v>
-      </c>
-      <c r="B35" t="s">
-        <v>9</v>
-      </c>
-      <c r="C35" t="s">
-        <v>9</v>
-      </c>
-      <c r="D35" t="s">
-        <v>21</v>
-      </c>
-      <c r="E35" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>40</v>
-      </c>
-      <c r="B36" t="s">
-        <v>9</v>
-      </c>
-      <c r="C36" t="s">
-        <v>9</v>
-      </c>
-      <c r="D36" t="s">
-        <v>21</v>
-      </c>
-      <c r="E36" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>41</v>
-      </c>
-      <c r="B37" t="s">
-        <v>9</v>
-      </c>
-      <c r="C37" t="s">
-        <v>9</v>
-      </c>
-      <c r="D37" t="s">
-        <v>21</v>
-      </c>
-      <c r="E37" t="s">
-        <v>180</v>
+      <c r="A34" s="2" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>42</v>
-      </c>
-      <c r="B38" t="s">
-        <v>9</v>
-      </c>
-      <c r="C38" t="s">
-        <v>9</v>
-      </c>
-      <c r="D38" t="s">
-        <v>21</v>
-      </c>
-      <c r="E38" t="s">
-        <v>180</v>
-      </c>
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B39" t="s">
         <v>9</v>
@@ -1514,12 +1984,12 @@
         <v>21</v>
       </c>
       <c r="E39" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B40" t="s">
         <v>9</v>
@@ -1531,12 +2001,12 @@
         <v>21</v>
       </c>
       <c r="E40" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B41" t="s">
         <v>9</v>
@@ -1548,12 +2018,12 @@
         <v>21</v>
       </c>
       <c r="E41" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B42" t="s">
         <v>9</v>
@@ -1565,12 +2035,12 @@
         <v>21</v>
       </c>
       <c r="E42" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B43" t="s">
         <v>9</v>
@@ -1582,12 +2052,12 @@
         <v>21</v>
       </c>
       <c r="E43" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B44" t="s">
         <v>9</v>
@@ -1599,12 +2069,12 @@
         <v>21</v>
       </c>
       <c r="E44" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B45" t="s">
         <v>9</v>
@@ -1616,12 +2086,12 @@
         <v>21</v>
       </c>
       <c r="E45" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B46" t="s">
         <v>9</v>
@@ -1633,12 +2103,12 @@
         <v>21</v>
       </c>
       <c r="E46" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B47" t="s">
         <v>9</v>
@@ -1650,12 +2120,12 @@
         <v>21</v>
       </c>
       <c r="E47" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B48" t="s">
         <v>9</v>
@@ -1667,12 +2137,12 @@
         <v>21</v>
       </c>
       <c r="E48" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B49" t="s">
         <v>9</v>
@@ -1684,12 +2154,12 @@
         <v>21</v>
       </c>
       <c r="E49" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B50" t="s">
         <v>9</v>
@@ -1701,12 +2171,12 @@
         <v>21</v>
       </c>
       <c r="E50" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B51" t="s">
         <v>9</v>
@@ -1718,12 +2188,12 @@
         <v>21</v>
       </c>
       <c r="E51" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B52" t="s">
         <v>9</v>
@@ -1735,12 +2205,12 @@
         <v>21</v>
       </c>
       <c r="E52" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B53" t="s">
         <v>9</v>
@@ -1752,12 +2222,12 @@
         <v>21</v>
       </c>
       <c r="E53" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B54" t="s">
         <v>9</v>
@@ -1769,12 +2239,12 @@
         <v>21</v>
       </c>
       <c r="E54" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B55" t="s">
         <v>9</v>
@@ -1786,12 +2256,12 @@
         <v>21</v>
       </c>
       <c r="E55" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B56" t="s">
         <v>9</v>
@@ -1803,12 +2273,12 @@
         <v>21</v>
       </c>
       <c r="E56" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B57" t="s">
         <v>9</v>
@@ -1820,12 +2290,12 @@
         <v>21</v>
       </c>
       <c r="E57" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B58" t="s">
         <v>9</v>
@@ -1837,12 +2307,12 @@
         <v>21</v>
       </c>
       <c r="E58" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B59" t="s">
         <v>9</v>
@@ -1854,12 +2324,12 @@
         <v>21</v>
       </c>
       <c r="E59" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B60" t="s">
         <v>9</v>
@@ -1871,12 +2341,12 @@
         <v>21</v>
       </c>
       <c r="E60" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B61" t="s">
         <v>9</v>
@@ -1888,12 +2358,12 @@
         <v>21</v>
       </c>
       <c r="E61" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B62" t="s">
         <v>9</v>
@@ -1905,12 +2375,12 @@
         <v>21</v>
       </c>
       <c r="E62" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B63" t="s">
         <v>9</v>
@@ -1922,12 +2392,12 @@
         <v>21</v>
       </c>
       <c r="E63" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B64" t="s">
         <v>9</v>
@@ -1939,12 +2409,12 @@
         <v>21</v>
       </c>
       <c r="E64" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="B65" t="s">
         <v>9</v>
@@ -1956,12 +2426,12 @@
         <v>21</v>
       </c>
       <c r="E65" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B66" t="s">
         <v>9</v>
@@ -1973,12 +2443,12 @@
         <v>21</v>
       </c>
       <c r="E66" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B67" t="s">
         <v>9</v>
@@ -1990,12 +2460,12 @@
         <v>21</v>
       </c>
       <c r="E67" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B68" t="s">
         <v>9</v>
@@ -2007,12 +2477,12 @@
         <v>21</v>
       </c>
       <c r="E68" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B69" t="s">
         <v>9</v>
@@ -2024,12 +2494,12 @@
         <v>21</v>
       </c>
       <c r="E69" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B70" t="s">
         <v>9</v>
@@ -2041,12 +2511,12 @@
         <v>21</v>
       </c>
       <c r="E70" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B71" t="s">
         <v>9</v>
@@ -2058,12 +2528,12 @@
         <v>21</v>
       </c>
       <c r="E71" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B72" t="s">
         <v>9</v>
@@ -2075,12 +2545,12 @@
         <v>21</v>
       </c>
       <c r="E72" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B73" t="s">
         <v>9</v>
@@ -2092,12 +2562,12 @@
         <v>21</v>
       </c>
       <c r="E73" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B74" t="s">
         <v>9</v>
@@ -2109,12 +2579,12 @@
         <v>21</v>
       </c>
       <c r="E74" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B75" t="s">
         <v>9</v>
@@ -2126,12 +2596,12 @@
         <v>21</v>
       </c>
       <c r="E75" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B76" t="s">
         <v>9</v>
@@ -2143,12 +2613,12 @@
         <v>21</v>
       </c>
       <c r="E76" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B77" t="s">
         <v>9</v>
@@ -2160,12 +2630,12 @@
         <v>21</v>
       </c>
       <c r="E77" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B78" t="s">
         <v>9</v>
@@ -2177,12 +2647,12 @@
         <v>21</v>
       </c>
       <c r="E78" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B79" t="s">
         <v>9</v>
@@ -2194,12 +2664,12 @@
         <v>21</v>
       </c>
       <c r="E79" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B80" t="s">
         <v>9</v>
@@ -2211,12 +2681,12 @@
         <v>21</v>
       </c>
       <c r="E80" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B81" t="s">
         <v>9</v>
@@ -2228,12 +2698,12 @@
         <v>21</v>
       </c>
       <c r="E81" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B82" t="s">
         <v>9</v>
@@ -2245,12 +2715,12 @@
         <v>21</v>
       </c>
       <c r="E82" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B83" t="s">
         <v>9</v>
@@ -2262,12 +2732,12 @@
         <v>21</v>
       </c>
       <c r="E83" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B84" t="s">
         <v>9</v>
@@ -2279,12 +2749,12 @@
         <v>21</v>
       </c>
       <c r="E84" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B85" t="s">
         <v>9</v>
@@ -2296,12 +2766,12 @@
         <v>21</v>
       </c>
       <c r="E85" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B86" t="s">
         <v>9</v>
@@ -2313,12 +2783,12 @@
         <v>21</v>
       </c>
       <c r="E86" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B87" t="s">
         <v>9</v>
@@ -2330,12 +2800,12 @@
         <v>21</v>
       </c>
       <c r="E87" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B88" t="s">
         <v>9</v>
@@ -2347,12 +2817,12 @@
         <v>21</v>
       </c>
       <c r="E88" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="B89" t="s">
         <v>9</v>
@@ -2364,12 +2834,12 @@
         <v>21</v>
       </c>
       <c r="E89" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B90" t="s">
         <v>9</v>
@@ -2381,12 +2851,12 @@
         <v>21</v>
       </c>
       <c r="E90" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B91" t="s">
         <v>9</v>
@@ -2398,12 +2868,12 @@
         <v>21</v>
       </c>
       <c r="E91" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B92" t="s">
         <v>9</v>
@@ -2415,12 +2885,12 @@
         <v>21</v>
       </c>
       <c r="E92" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B93" t="s">
         <v>9</v>
@@ -2432,12 +2902,12 @@
         <v>21</v>
       </c>
       <c r="E93" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B94" t="s">
         <v>9</v>
@@ -2449,12 +2919,12 @@
         <v>21</v>
       </c>
       <c r="E94" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B95" t="s">
         <v>9</v>
@@ -2466,12 +2936,12 @@
         <v>21</v>
       </c>
       <c r="E95" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B96" t="s">
         <v>9</v>
@@ -2483,12 +2953,12 @@
         <v>21</v>
       </c>
       <c r="E96" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B97" t="s">
         <v>9</v>
@@ -2500,12 +2970,12 @@
         <v>21</v>
       </c>
       <c r="E97" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B98" t="s">
         <v>9</v>
@@ -2517,12 +2987,12 @@
         <v>21</v>
       </c>
       <c r="E98" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B99" t="s">
         <v>9</v>
@@ -2534,12 +3004,12 @@
         <v>21</v>
       </c>
       <c r="E99" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B100" t="s">
         <v>9</v>
@@ -2551,12 +3021,12 @@
         <v>21</v>
       </c>
       <c r="E100" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="B101" t="s">
         <v>9</v>
@@ -2568,12 +3038,12 @@
         <v>21</v>
       </c>
       <c r="E101" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B102" t="s">
         <v>9</v>
@@ -2585,12 +3055,12 @@
         <v>21</v>
       </c>
       <c r="E102" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="B103" t="s">
         <v>9</v>
@@ -2602,12 +3072,12 @@
         <v>21</v>
       </c>
       <c r="E103" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B104" t="s">
         <v>9</v>
@@ -2619,12 +3089,12 @@
         <v>21</v>
       </c>
       <c r="E104" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B105" t="s">
         <v>9</v>
@@ -2636,12 +3106,12 @@
         <v>21</v>
       </c>
       <c r="E105" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="B106" t="s">
         <v>9</v>
@@ -2653,12 +3123,12 @@
         <v>21</v>
       </c>
       <c r="E106" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B107" t="s">
         <v>9</v>
@@ -2670,12 +3140,12 @@
         <v>21</v>
       </c>
       <c r="E107" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B108" t="s">
         <v>9</v>
@@ -2687,12 +3157,12 @@
         <v>21</v>
       </c>
       <c r="E108" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B109" t="s">
         <v>9</v>
@@ -2704,12 +3174,12 @@
         <v>21</v>
       </c>
       <c r="E109" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="B110" t="s">
         <v>9</v>
@@ -2721,12 +3191,12 @@
         <v>21</v>
       </c>
       <c r="E110" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="B111" t="s">
         <v>9</v>
@@ -2738,12 +3208,12 @@
         <v>21</v>
       </c>
       <c r="E111" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B112" t="s">
         <v>9</v>
@@ -2755,12 +3225,12 @@
         <v>21</v>
       </c>
       <c r="E112" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B113" t="s">
         <v>9</v>
@@ -2772,12 +3242,12 @@
         <v>21</v>
       </c>
       <c r="E113" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="B114" t="s">
         <v>9</v>
@@ -2789,12 +3259,12 @@
         <v>21</v>
       </c>
       <c r="E114" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B115" t="s">
         <v>9</v>
@@ -2806,12 +3276,12 @@
         <v>21</v>
       </c>
       <c r="E115" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B116" t="s">
         <v>9</v>
@@ -2823,12 +3293,12 @@
         <v>21</v>
       </c>
       <c r="E116" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B117" t="s">
         <v>9</v>
@@ -2840,12 +3310,12 @@
         <v>21</v>
       </c>
       <c r="E117" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B118" t="s">
         <v>9</v>
@@ -2857,12 +3327,12 @@
         <v>21</v>
       </c>
       <c r="E118" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B119" t="s">
         <v>9</v>
@@ -2874,12 +3344,12 @@
         <v>21</v>
       </c>
       <c r="E119" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="B120" t="s">
         <v>9</v>
@@ -2891,12 +3361,12 @@
         <v>21</v>
       </c>
       <c r="E120" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B121" t="s">
         <v>9</v>
@@ -2908,12 +3378,12 @@
         <v>21</v>
       </c>
       <c r="E121" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B122" t="s">
         <v>9</v>
@@ -2925,12 +3395,12 @@
         <v>21</v>
       </c>
       <c r="E122" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B123" t="s">
         <v>9</v>
@@ -2942,12 +3412,12 @@
         <v>21</v>
       </c>
       <c r="E123" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B124" t="s">
         <v>9</v>
@@ -2959,12 +3429,12 @@
         <v>21</v>
       </c>
       <c r="E124" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="B125" t="s">
         <v>9</v>
@@ -2976,12 +3446,12 @@
         <v>21</v>
       </c>
       <c r="E125" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="B126" t="s">
         <v>9</v>
@@ -2993,12 +3463,12 @@
         <v>21</v>
       </c>
       <c r="E126" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="B127" t="s">
         <v>9</v>
@@ -3010,12 +3480,12 @@
         <v>21</v>
       </c>
       <c r="E127" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B128" t="s">
         <v>9</v>
@@ -3027,12 +3497,12 @@
         <v>21</v>
       </c>
       <c r="E128" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="B129" t="s">
         <v>9</v>
@@ -3044,12 +3514,12 @@
         <v>21</v>
       </c>
       <c r="E129" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="B130" t="s">
         <v>9</v>
@@ -3061,12 +3531,12 @@
         <v>21</v>
       </c>
       <c r="E130" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="B131" t="s">
         <v>9</v>
@@ -3078,12 +3548,12 @@
         <v>21</v>
       </c>
       <c r="E131" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="B132" t="s">
         <v>9</v>
@@ -3095,12 +3565,12 @@
         <v>21</v>
       </c>
       <c r="E132" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="B133" t="s">
         <v>9</v>
@@ -3112,12 +3582,12 @@
         <v>21</v>
       </c>
       <c r="E133" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="B134" t="s">
         <v>9</v>
@@ -3129,12 +3599,12 @@
         <v>21</v>
       </c>
       <c r="E134" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B135" t="s">
         <v>9</v>
@@ -3146,12 +3616,12 @@
         <v>21</v>
       </c>
       <c r="E135" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="B136" t="s">
         <v>9</v>
@@ -3163,12 +3633,12 @@
         <v>21</v>
       </c>
       <c r="E136" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="B137" t="s">
         <v>9</v>
@@ -3180,12 +3650,12 @@
         <v>21</v>
       </c>
       <c r="E137" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B138" t="s">
         <v>9</v>
@@ -3197,12 +3667,12 @@
         <v>21</v>
       </c>
       <c r="E138" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="B139" t="s">
         <v>9</v>
@@ -3214,12 +3684,12 @@
         <v>21</v>
       </c>
       <c r="E139" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="B140" t="s">
         <v>9</v>
@@ -3231,12 +3701,12 @@
         <v>21</v>
       </c>
       <c r="E140" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="B141" t="s">
         <v>9</v>
@@ -3248,12 +3718,12 @@
         <v>21</v>
       </c>
       <c r="E141" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="B142" t="s">
         <v>9</v>
@@ -3265,12 +3735,12 @@
         <v>21</v>
       </c>
       <c r="E142" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="B143" t="s">
         <v>9</v>
@@ -3282,12 +3752,12 @@
         <v>21</v>
       </c>
       <c r="E143" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="B144" t="s">
         <v>9</v>
@@ -3299,12 +3769,12 @@
         <v>21</v>
       </c>
       <c r="E144" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="B145" t="s">
         <v>9</v>
@@ -3316,12 +3786,12 @@
         <v>21</v>
       </c>
       <c r="E145" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="B146" t="s">
         <v>9</v>
@@ -3333,12 +3803,12 @@
         <v>21</v>
       </c>
       <c r="E146" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="B147" t="s">
         <v>9</v>
@@ -3350,12 +3820,12 @@
         <v>21</v>
       </c>
       <c r="E147" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="B148" t="s">
         <v>9</v>
@@ -3367,12 +3837,12 @@
         <v>21</v>
       </c>
       <c r="E148" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="B149" t="s">
         <v>9</v>
@@ -3384,21 +3854,63 @@
         <v>21</v>
       </c>
       <c r="E149" t="s">
-        <v>180</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
+        <v>146</v>
+      </c>
+      <c r="B150" t="s">
+        <v>9</v>
+      </c>
+      <c r="C150" t="s">
+        <v>9</v>
+      </c>
+      <c r="D150" t="s">
+        <v>21</v>
+      </c>
+      <c r="E150" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>147</v>
+      </c>
+      <c r="B151" t="s">
+        <v>9</v>
+      </c>
+      <c r="C151" t="s">
+        <v>9</v>
+      </c>
+      <c r="D151" t="s">
+        <v>21</v>
+      </c>
+      <c r="E151" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A152" s="1"/>
-      <c r="B152" s="1"/>
-      <c r="C152" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D152" s="1"/>
-      <c r="E152" s="1"/>
+      <c r="A152" t="s">
+        <v>148</v>
+      </c>
+      <c r="B152" t="s">
+        <v>9</v>
+      </c>
+      <c r="C152" t="s">
+        <v>9</v>
+      </c>
+      <c r="D152" t="s">
+        <v>21</v>
+      </c>
+      <c r="E152" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="B153" t="s">
         <v>9</v>
@@ -3407,15 +3919,15 @@
         <v>9</v>
       </c>
       <c r="D153" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E153" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="B154" t="s">
         <v>9</v>
@@ -3424,15 +3936,15 @@
         <v>9</v>
       </c>
       <c r="D154" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E154" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B155" t="s">
         <v>9</v>
@@ -3441,15 +3953,15 @@
         <v>9</v>
       </c>
       <c r="D155" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E155" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B156" t="s">
         <v>9</v>
@@ -3458,15 +3970,15 @@
         <v>9</v>
       </c>
       <c r="D156" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E156" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="B157" t="s">
         <v>9</v>
@@ -3475,100 +3987,29 @@
         <v>9</v>
       </c>
       <c r="D157" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E157" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A158" t="s">
-        <v>162</v>
-      </c>
-      <c r="B158" t="s">
-        <v>9</v>
-      </c>
-      <c r="C158" t="s">
-        <v>9</v>
-      </c>
-      <c r="D158" t="s">
-        <v>12</v>
-      </c>
-      <c r="E158" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A159" t="s">
-        <v>163</v>
-      </c>
-      <c r="B159" t="s">
-        <v>9</v>
-      </c>
-      <c r="C159" t="s">
-        <v>9</v>
-      </c>
-      <c r="D159" t="s">
-        <v>12</v>
-      </c>
-      <c r="E159" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A160" t="s">
-        <v>164</v>
-      </c>
-      <c r="B160" t="s">
-        <v>9</v>
-      </c>
-      <c r="C160" t="s">
-        <v>9</v>
-      </c>
-      <c r="D160" t="s">
-        <v>12</v>
-      </c>
-      <c r="E160" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A161" t="s">
-        <v>165</v>
-      </c>
-      <c r="B161" t="s">
-        <v>9</v>
-      </c>
-      <c r="C161" t="s">
-        <v>9</v>
-      </c>
-      <c r="D161" t="s">
-        <v>12</v>
-      </c>
-      <c r="E161" t="s">
-        <v>180</v>
+      <c r="A158" s="2" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A162" t="s">
-        <v>166</v>
-      </c>
-      <c r="B162" t="s">
-        <v>9</v>
-      </c>
-      <c r="C162" t="s">
-        <v>9</v>
-      </c>
-      <c r="D162" t="s">
-        <v>12</v>
-      </c>
-      <c r="E162" t="s">
-        <v>180</v>
-      </c>
+      <c r="A162" s="1"/>
+      <c r="B162" s="1"/>
+      <c r="C162" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D162" s="1"/>
+      <c r="E162" s="1"/>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="B163" t="s">
         <v>9</v>
@@ -3580,12 +4021,12 @@
         <v>12</v>
       </c>
       <c r="E163" t="s">
-        <v>180</v>
+        <v>12</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="B164" t="s">
         <v>9</v>
@@ -3597,12 +4038,12 @@
         <v>12</v>
       </c>
       <c r="E164" t="s">
-        <v>180</v>
+        <v>12</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="B165" t="s">
         <v>9</v>
@@ -3614,12 +4055,12 @@
         <v>12</v>
       </c>
       <c r="E165" t="s">
-        <v>180</v>
+        <v>12</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="B166" t="s">
         <v>9</v>
@@ -3631,12 +4072,12 @@
         <v>12</v>
       </c>
       <c r="E166" t="s">
-        <v>180</v>
+        <v>12</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="B167" t="s">
         <v>9</v>
@@ -3648,12 +4089,12 @@
         <v>12</v>
       </c>
       <c r="E167" t="s">
-        <v>180</v>
+        <v>12</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="B168" t="s">
         <v>9</v>
@@ -3665,12 +4106,12 @@
         <v>12</v>
       </c>
       <c r="E168" t="s">
-        <v>180</v>
+        <v>12</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="B169" t="s">
         <v>9</v>
@@ -3682,12 +4123,12 @@
         <v>12</v>
       </c>
       <c r="E169" t="s">
-        <v>180</v>
+        <v>12</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="B170" t="s">
         <v>9</v>
@@ -3699,12 +4140,12 @@
         <v>12</v>
       </c>
       <c r="E170" t="s">
-        <v>180</v>
+        <v>12</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="B171" t="s">
         <v>9</v>
@@ -3716,12 +4157,12 @@
         <v>12</v>
       </c>
       <c r="E171" t="s">
-        <v>180</v>
+        <v>12</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="B172" t="s">
         <v>9</v>
@@ -3733,12 +4174,12 @@
         <v>12</v>
       </c>
       <c r="E172" t="s">
-        <v>180</v>
+        <v>12</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="B173" t="s">
         <v>9</v>
@@ -3750,12 +4191,12 @@
         <v>12</v>
       </c>
       <c r="E173" t="s">
-        <v>180</v>
+        <v>12</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="B174" t="s">
         <v>9</v>
@@ -3767,28 +4208,337 @@
         <v>12</v>
       </c>
       <c r="E174" t="s">
-        <v>180</v>
+        <v>12</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
+        <v>169</v>
+      </c>
+      <c r="B175" t="s">
+        <v>9</v>
+      </c>
+      <c r="C175" t="s">
+        <v>9</v>
+      </c>
+      <c r="D175" t="s">
+        <v>12</v>
+      </c>
+      <c r="E175" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A176" t="s">
+        <v>170</v>
+      </c>
+      <c r="B176" t="s">
+        <v>9</v>
+      </c>
+      <c r="C176" t="s">
+        <v>9</v>
+      </c>
+      <c r="D176" t="s">
+        <v>12</v>
+      </c>
+      <c r="E176" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A177" t="s">
+        <v>171</v>
+      </c>
+      <c r="B177" t="s">
+        <v>9</v>
+      </c>
+      <c r="C177" t="s">
+        <v>9</v>
+      </c>
+      <c r="D177" t="s">
+        <v>12</v>
+      </c>
+      <c r="E177" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A178" t="s">
+        <v>172</v>
+      </c>
+      <c r="B178" t="s">
+        <v>9</v>
+      </c>
+      <c r="C178" t="s">
+        <v>9</v>
+      </c>
+      <c r="D178" t="s">
+        <v>12</v>
+      </c>
+      <c r="E178" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A179" t="s">
+        <v>173</v>
+      </c>
+      <c r="B179" t="s">
+        <v>9</v>
+      </c>
+      <c r="C179" t="s">
+        <v>9</v>
+      </c>
+      <c r="D179" t="s">
+        <v>12</v>
+      </c>
+      <c r="E179" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A180" t="s">
+        <v>174</v>
+      </c>
+      <c r="B180" t="s">
+        <v>9</v>
+      </c>
+      <c r="C180" t="s">
+        <v>9</v>
+      </c>
+      <c r="D180" t="s">
+        <v>12</v>
+      </c>
+      <c r="E180" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A181" t="s">
+        <v>175</v>
+      </c>
+      <c r="B181" t="s">
+        <v>9</v>
+      </c>
+      <c r="C181" t="s">
+        <v>9</v>
+      </c>
+      <c r="D181" t="s">
+        <v>12</v>
+      </c>
+      <c r="E181" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A182" t="s">
+        <v>176</v>
+      </c>
+      <c r="B182" t="s">
+        <v>9</v>
+      </c>
+      <c r="C182" t="s">
+        <v>9</v>
+      </c>
+      <c r="D182" t="s">
+        <v>12</v>
+      </c>
+      <c r="E182" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A183" t="s">
+        <v>177</v>
+      </c>
+      <c r="B183" t="s">
+        <v>9</v>
+      </c>
+      <c r="C183" t="s">
+        <v>9</v>
+      </c>
+      <c r="D183" t="s">
+        <v>12</v>
+      </c>
+      <c r="E183" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A184" t="s">
+        <v>178</v>
+      </c>
+      <c r="B184" t="s">
+        <v>9</v>
+      </c>
+      <c r="C184" t="s">
+        <v>9</v>
+      </c>
+      <c r="D184" t="s">
+        <v>12</v>
+      </c>
+      <c r="E184" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A185" t="s">
         <v>179</v>
       </c>
-      <c r="B175" t="s">
-        <v>9</v>
-      </c>
-      <c r="C175" t="s">
-        <v>9</v>
-      </c>
-      <c r="D175" t="s">
-        <v>12</v>
-      </c>
-      <c r="E175" t="s">
+      <c r="B185" t="s">
+        <v>9</v>
+      </c>
+      <c r="C185" t="s">
+        <v>9</v>
+      </c>
+      <c r="D185" t="s">
+        <v>12</v>
+      </c>
+      <c r="E185" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A186" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A190" s="1"/>
+      <c r="B190" s="1"/>
+      <c r="C190" s="1" t="s">
         <v>180</v>
+      </c>
+      <c r="D190" s="1"/>
+      <c r="E190" s="1"/>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A191" t="s">
+        <v>2</v>
+      </c>
+      <c r="B191" t="s">
+        <v>9</v>
+      </c>
+      <c r="C191" t="s">
+        <v>181</v>
+      </c>
+      <c r="D191" t="s">
+        <v>12</v>
+      </c>
+      <c r="E191" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A192" t="s">
+        <v>3</v>
+      </c>
+      <c r="B192" t="s">
+        <v>9</v>
+      </c>
+      <c r="C192" t="s">
+        <v>181</v>
+      </c>
+      <c r="D192" t="s">
+        <v>12</v>
+      </c>
+      <c r="E192" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A193" t="s">
+        <v>4</v>
+      </c>
+      <c r="B193" t="s">
+        <v>9</v>
+      </c>
+      <c r="C193" t="s">
+        <v>181</v>
+      </c>
+      <c r="D193" t="s">
+        <v>12</v>
+      </c>
+      <c r="E193" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A194" t="s">
+        <v>5</v>
+      </c>
+      <c r="B194" t="s">
+        <v>9</v>
+      </c>
+      <c r="C194" t="s">
+        <v>181</v>
+      </c>
+      <c r="D194" t="s">
+        <v>12</v>
+      </c>
+      <c r="E194" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A195" t="s">
+        <v>6</v>
+      </c>
+      <c r="B195" t="s">
+        <v>9</v>
+      </c>
+      <c r="C195" t="s">
+        <v>181</v>
+      </c>
+      <c r="D195" t="s">
+        <v>12</v>
+      </c>
+      <c r="E195" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A196" t="s">
+        <v>7</v>
+      </c>
+      <c r="B196" t="s">
+        <v>9</v>
+      </c>
+      <c r="C196" t="s">
+        <v>181</v>
+      </c>
+      <c r="D196" t="s">
+        <v>12</v>
+      </c>
+      <c r="E196" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A197" t="s">
+        <v>8</v>
+      </c>
+      <c r="B197" t="s">
+        <v>9</v>
+      </c>
+      <c r="C197" t="s">
+        <v>181</v>
+      </c>
+      <c r="D197" t="s">
+        <v>12</v>
+      </c>
+      <c r="E197" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A198" s="2" t="s">
+        <v>184</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>